<commit_message>
added new classes and tests
</commit_message>
<xml_diff>
--- a/src/test/java/users.xlsx
+++ b/src/test/java/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steva\FinalProjectPOM\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFCF7EC-AF47-4BF3-B5E2-D4D3EAD7C6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC1FD53-C2EB-4ED9-BC6C-C017885D9A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="444" windowWidth="22440" windowHeight="12516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="444" windowWidth="22428" windowHeight="12516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Valid username</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>perfection_password</t>
+  </si>
+  <si>
+    <t>Error_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
   </si>
 </sst>
 </file>
@@ -469,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,9 +490,10 @@
     <col min="5" max="5" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,8 +515,11 @@
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -531,8 +541,11 @@
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -545,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -558,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -571,7 +584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -584,7 +597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -597,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
@@ -605,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
@@ -613,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>26</v>
       </c>
@@ -621,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>28</v>
       </c>
@@ -629,7 +642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>